<commit_message>
removed afo, cheminf otw, changed references in pid article, updated table in LbE, further minor fixes in mcrs and ctfiles articles
</commit_message>
<xml_diff>
--- a/static/assets/Supplementary_table_template.xlsx
+++ b/static/assets/Supplementary_table_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8757AEC8-9BEC-48B5-8285-3C9068FBBBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E1E4C0-B0E9-4414-8B0F-9392ED2E400B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12240" windowWidth="29040" windowHeight="15990" xr2:uid="{24EC6C05-62EA-4644-B615-EC0B700F9E64}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>SMILES</t>
   </si>
@@ -97,18 +97,6 @@
     <t>Ontology_URL</t>
   </si>
   <si>
-    <t>http://purl.allotrope.org/ontologies/result#AFR_0001118</t>
-  </si>
-  <si>
-    <t>AFR:0001118</t>
-  </si>
-  <si>
-    <t>http://purl.allotrope.org/ontologies/result#AFR_0000919</t>
-  </si>
-  <si>
-    <t>AFR:0000919</t>
-  </si>
-  <si>
     <t>&lt;DOI of dataset&gt;</t>
   </si>
   <si>
@@ -128,12 +116,6 @@
   </si>
   <si>
     <t>IUPAC name</t>
-  </si>
-  <si>
-    <t>local identifier</t>
-  </si>
-  <si>
-    <t>sample identifier</t>
   </si>
   <si>
     <t>Lettercode_number_lab_journal</t>
@@ -587,7 +569,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,13 +589,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
@@ -642,37 +624,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1"/>
     </row>
@@ -680,12 +656,6 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
@@ -693,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
@@ -716,12 +686,6 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
@@ -729,10 +693,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>16</v>
@@ -753,31 +717,31 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I5">
         <v>7410</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="L5" s="1"/>
     </row>
@@ -786,28 +750,28 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I6">
         <v>5950</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -816,31 +780,31 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I7">
         <v>3034034</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="L7" s="1"/>
     </row>

</xml_diff>

<commit_message>
feat: added missing ontology links to supp table
</commit_message>
<xml_diff>
--- a/static/assets/Supplementary_table_template.xlsx
+++ b/static/assets/Supplementary_table_template.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A355411E-8CD8-4349-9602-F3621FF8D7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD45563D-181A-4EB2-99DA-E8E95477108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8640" windowWidth="29040" windowHeight="17790" xr2:uid="{24EC6C05-62EA-4644-B615-EC0B700F9E64}"/>
+    <workbookView xWindow="-28920" yWindow="-225" windowWidth="29040" windowHeight="17520" xr2:uid="{24EC6C05-62EA-4644-B615-EC0B700F9E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,47 +29,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t>InChIKey</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>http://semanticscience.org/resource/CHEMINF_000107</t>
   </si>
   <si>
-    <t>http://semanticscience.org/resource/SIO_000122</t>
-  </si>
-  <si>
     <t>http://semanticscience.org/resource/CHEMINF_000059</t>
   </si>
   <si>
-    <t>http://semanticscience.org/resource/CHEMINF_000140</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/CHEMINF_000446</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>CAS registry number</t>
-  </si>
-  <si>
-    <t>PubChem compound identifier (CID)</t>
-  </si>
-  <si>
-    <t>synonym</t>
-  </si>
-  <si>
     <t>IUPAC name</t>
   </si>
   <si>
     <t>1-phenylethanone</t>
   </si>
   <si>
-    <t>acetophenone</t>
-  </si>
-  <si>
     <t>CC(C1=CC=CC=C1)=O</t>
   </si>
   <si>
@@ -80,15 +52,9 @@
     <t>KWOLFJPFCHCOCG-UHFFFAOYSA-N</t>
   </si>
   <si>
-    <t>98-86-2</t>
-  </si>
-  <si>
     <t>(2S)-2-aminopropanoic acid</t>
   </si>
   <si>
-    <t>alanine</t>
-  </si>
-  <si>
     <t>N[C@@H](C)C(O)=O</t>
   </si>
   <si>
@@ -98,15 +64,9 @@
     <t>QNAYBMKLOCPYGJ-REOHCLBHSA-N</t>
   </si>
   <si>
-    <t>56-41-7</t>
-  </si>
-  <si>
     <t>(R)-[(2S,4S,5R)-5-ethenyl-1-azabicyclo[2.2.2]octan-2-yl]-(6-methoxyquinolin-4-yl)methanol</t>
   </si>
   <si>
-    <t>quinine</t>
-  </si>
-  <si>
     <t>[H][C@@]1([C@@H](C2=CC=NC3=CC=C(C=C23)OC)O)C[C@@H]4CC[N@]1C[C@@H]4C=C</t>
   </si>
   <si>
@@ -116,9 +76,6 @@
     <t>LOUPRKONTZGTKE-WZBLMQSHSA-N</t>
   </si>
   <si>
-    <t>72402-53-0</t>
-  </si>
-  <si>
     <t>NFDI-0007</t>
   </si>
   <si>
@@ -128,12 +85,6 @@
     <t>NFDI-1245</t>
   </si>
   <si>
-    <t>from cinchona tree</t>
-  </si>
-  <si>
-    <t>from labdanum</t>
-  </si>
-  <si>
     <t>http://semanticscience.org/resource/CHEMINF_000018</t>
   </si>
   <si>
@@ -143,22 +94,28 @@
     <t>http://semanticscience.org/resource/CHEMINF_000113</t>
   </si>
   <si>
-    <t>InChI descriptor</t>
-  </si>
-  <si>
     <t>IRI</t>
   </si>
   <si>
     <t>Label</t>
   </si>
   <si>
-    <t>http://semanticscience.org/resource/SIO_001167</t>
-  </si>
-  <si>
-    <t>Local chemical structure identifier</t>
-  </si>
-  <si>
-    <t>local chemical sample symbol</t>
+    <t>InChI Identifier</t>
+  </si>
+  <si>
+    <t>InChIKey Identifier</t>
+  </si>
+  <si>
+    <t>http://purl.allotrope.org/ontologies/result#AFR_0000919</t>
+  </si>
+  <si>
+    <t>http://purl.allotrope.org/ontologies/result#AFR_0001118</t>
+  </si>
+  <si>
+    <t>Local structure identifier in article</t>
+  </si>
+  <si>
+    <t>Local identifier of a sample measured</t>
   </si>
 </sst>
 </file>
@@ -182,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -190,15 +147,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,230 +482,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430A3A8D-DC73-4805-8C6B-1B7DBA4F6177}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="8" width="24.21875" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" customWidth="1"/>
-    <col min="10" max="10" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3">
-        <v>7410</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4">
-        <v>5950</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5">
-        <v>3034034</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: added placeholder for DOI of dataset
</commit_message>
<xml_diff>
--- a/static/assets/Supplementary_table_template.xlsx
+++ b/static/assets/Supplementary_table_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD45563D-181A-4EB2-99DA-E8E95477108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E5E76C-1C6A-410E-9B64-CE1A692CAEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-225" windowWidth="29040" windowHeight="17520" xr2:uid="{24EC6C05-62EA-4644-B615-EC0B700F9E64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24EC6C05-62EA-4644-B615-EC0B700F9E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>http://semanticscience.org/resource/CHEMINF_000107</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Local identifier of a sample measured</t>
+  </si>
+  <si>
+    <t>[DOI of dataset]</t>
   </si>
 </sst>
 </file>
@@ -485,21 +488,21 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -522,7 +525,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -545,7 +548,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
       <c r="B3">
         <v>1</v>
       </c>
@@ -565,10 +571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>20</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -585,9 +588,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -605,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -613,7 +616,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -621,7 +624,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -629,7 +632,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>

</xml_diff>